<commit_message>
Generalize name resolution so eval works.
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5744D39F-A903-4946-95D8-70FA94545439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE4EF49-7F4C-42DC-9FE2-49FB2D7E885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ALLOWEDTOTAL">Sheet2!$B$8</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>=1+1</t>
   </si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t>OK?</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -447,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -900,4 +910,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f>SUM(A2:B4)</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
date functions and user def fns
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE4EF49-7F4C-42DC-9FE2-49FB2D7E885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F5603C-9C36-4B07-B5B9-93F9368BA7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,10 +13,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ALLOWEDTOTAL">Sheet2!$B$8</definedName>
-    <definedName name="BONUS">Sheet2!$B$7</definedName>
-    <definedName name="EMPLOYEES">Sheet2!$A$2:$A$4</definedName>
-    <definedName name="WHATEVER">Sheet2!$E$6</definedName>
+    <definedName name="ALLOWEDTOTAL">Sheet2!$B$10</definedName>
+    <definedName name="BONUS">Sheet2!$B$9</definedName>
+    <definedName name="EMPLOYEES">Sheet2!$A$4:$A$6</definedName>
+    <definedName name="PREPDATE">Sheet2!$B$1</definedName>
+    <definedName name="WHATEVER">Sheet2!$H$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>=1+1</t>
   </si>
@@ -85,6 +86,39 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Perecentage</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Hired</t>
+  </si>
+  <si>
+    <t>Prepared</t>
+  </si>
+  <si>
+    <t>Tenure (Days)</t>
+  </si>
+  <si>
+    <t>Tenure (Years)</t>
   </si>
 </sst>
 </file>
@@ -134,13 +168,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,140 +805,238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525E6BAE-ADD8-5442-95D5-81931F206D16}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7">
+        <v>44437</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B4" s="7">
+        <v>43101</v>
+      </c>
+      <c r="C4" s="2">
+        <f>_xlfn.DAYS(PREPDATE,B4)</f>
+        <v>1336</v>
+      </c>
+      <c r="D4" s="3">
+        <f>YEARFRAC(PREPDATE,B4)</f>
+        <v>3.661111111111111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="C2" s="2">
-        <f>BONUS * B2</f>
+      <c r="H4" s="2">
+        <f>BONUS * G4</f>
         <v>12</v>
       </c>
-      <c r="D2">
+      <c r="I4">
         <v>6</v>
       </c>
-      <c r="E2">
-        <f>SUM(B2:D2)</f>
+      <c r="J4">
+        <f>SUM(G4:I4)</f>
         <v>118</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B5" s="7">
+        <v>44013</v>
+      </c>
+      <c r="C5" s="2">
+        <f>_xlfn.DAYS(PREPDATE,B5)</f>
+        <v>424</v>
+      </c>
+      <c r="D5" s="3">
+        <f>YEARFRAC(PREPDATE,B5,1)</f>
+        <v>1.1600547195622435</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
         <v>200</v>
       </c>
-      <c r="C3" s="2">
-        <f>BONUS * B3</f>
+      <c r="H5" s="2">
+        <f>BONUS * G5</f>
         <v>24</v>
       </c>
-      <c r="D3">
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">SUM(B3:D3)</f>
+      <c r="J5">
+        <f t="shared" ref="J5:J6" si="0">SUM(G5:I5)</f>
         <v>229</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B6" s="7">
+        <v>44075</v>
+      </c>
+      <c r="C6" s="2">
+        <f>_xlfn.DAYS(PREPDATE,B6)</f>
+        <v>362</v>
+      </c>
+      <c r="D6" s="3">
+        <f>YEARFRAC(PREPDATE,B6,3)</f>
+        <v>0.99178082191780825</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
         <v>300</v>
       </c>
-      <c r="C4" s="2">
-        <f>BONUS * B4</f>
+      <c r="H6" s="2">
+        <f>BONUS * G6</f>
         <v>36</v>
       </c>
-      <c r="D4">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>340</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <f>SUM(B2:B4)</f>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <f>SUM(G4:G6)</f>
         <v>600</v>
       </c>
-      <c r="C5">
-        <f t="shared" ref="C5:D5" si="1">SUM(C2:C4)</f>
+      <c r="H7">
+        <f t="shared" ref="H7:I7" si="1">SUM(H4:H6)</f>
         <v>72</v>
       </c>
-      <c r="D5">
+      <c r="I7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E5">
-        <f>SUM(E2:E4)</f>
+      <c r="J7">
+        <f>SUM(J4:J6)</f>
         <v>687</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6">
-        <f>SUM(B2:B4)-SUM(C2:C4)</f>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <f>SUM(G4:G6)-SUM(H4:H6)</f>
         <v>528</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B9" s="5">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <f>COUNTA(EMPLOYEES)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="str">
-        <f>IF(E5&lt;ALLOWEDTOTAL,"YES","NO")</f>
+      <c r="B13" t="str">
+        <f>IF(J7&lt;ALLOWEDTOTAL,"YES","NO")</f>
         <v>YES</v>
       </c>
     </row>
@@ -914,15 +1048,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -933,7 +1070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -941,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -949,7 +1086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -959,6 +1096,20 @@
       <c r="C4">
         <f>SUM(A2:B4)</f>
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f>_xlfn.DAYS(D9,E9)</f>
+        <v>-577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="7">
+        <v>43831</v>
+      </c>
+      <c r="E9" s="7">
+        <v>44408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Date parsing, DATEVALUE, correct YEARFRAC
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F5603C-9C36-4B07-B5B9-93F9368BA7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1122FC2E-CCC9-470E-8423-A0F0BB8F165E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
@@ -125,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +143,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -177,6 +184,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -797,6 +806,162 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <f>DATEVALUE("1/15/2021")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <f>DATEVALUE("2021/01/15")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <f>DATEVALUE("January 15, 2021")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <f>DATEVALUE("Jan 2021")</f>
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <f>DATEVALUE("1/15")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <f>DATEVALUE("Jan 15")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <f>DATEVALUE("JAN-15")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <f>DATEVALUE("Jan 2021")</f>
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <f>DATEVALUE("Jan 15, 2021")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <f>DATEVALUE("Jan2021")</f>
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <f>DATEVALUE("Jan15")</f>
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <f>DATEVALUE("01 Jan 1985")</f>
+        <v>31048</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <f>DATEVALUE("01 April 2020")</f>
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="e">
+        <f>DATEVALUE("XYZ 20")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="9">
+        <f>YEARFRAC("2001/01/25","2001/09/27")</f>
+        <v>0.67222222222222228</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="9">
+        <f>YEARFRAC("01/01/2018","12/31/2018")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="9">
+        <f>YEARFRAC("01/01/2018","07/31/2018")</f>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="8">
+        <f>YEARFRAC("1 Jan 20","1 April 2020",0)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="9">
+        <f>YEARFRAC("01 Jan 2020","01 April 2020",1)</f>
+        <v>0.24863387978142076</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="9">
+        <f>YEARFRAC("01 Jan 2020","02 Jan 2020",1)</f>
+        <v>2.7322404371584699E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="9">
+        <f>YEARFRAC("01 Jan 1985","02 Jan 1985",1)</f>
+        <v>2.7397260273972603E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="9">
+        <f>YEARFRAC("01 Jan 1985","01 April 2020",1)</f>
+        <v>35.247091033538673</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="9">
+        <f>YEARFRAC("01 Jan 2020","01 April 2020",1)</f>
+        <v>0.24863387978142076</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="9">
+        <f>YEARFRAC("01 Jan 2020","01 April 2020",2)</f>
+        <v>0.25277777777777777</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="9">
+        <f>YEARFRAC("01 Jan 2020","01 April 2020",3)</f>
+        <v>0.24931506849315069</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="9">
+        <f>YEARFRAC("01 Jan 2020","01 April 2020",4)</f>
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -808,7 +973,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1048,18 +1213,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1236,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1078,7 +1244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1086,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1098,17 +1264,104 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6">
         <f>_xlfn.DAYS(D9,E9)</f>
         <v>-577</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="7">
         <v>43831</v>
       </c>
       <c r="E9" s="7">
+        <v>44408</v>
+      </c>
+      <c r="G9">
+        <f>E9-D9</f>
+        <v>577</v>
+      </c>
+      <c r="H9">
+        <f>G9/360</f>
+        <v>1.6027777777777779</v>
+      </c>
+      <c r="J9">
+        <f>570/360</f>
+        <v>1.5833333333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>DATEDIF(D9,E9,"m")</f>
+        <v>18</v>
+      </c>
+      <c r="H10">
+        <f>G10*30</f>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f>YEARFRAC(D9,E9,0)</f>
+        <v>1.5833333333333333</v>
+      </c>
+      <c r="G11">
+        <f>DATEDIF(D9,E9,"y")</f>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f>H10+31</f>
+        <v>571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f>DATEDIF(D9,E9,"d")</f>
+        <v>577</v>
+      </c>
+      <c r="H12">
+        <f>H11/360</f>
+        <v>1.586111111111111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>DAY(D9)</f>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f>DAY(E9)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <f>MONTH(D9)</f>
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f>MONTH(E9)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>YEAR(D9)</f>
+        <v>2020</v>
+      </c>
+      <c r="H16">
+        <f>YEAR(E9)</f>
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="3">
+        <f>D9</f>
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="3">
         <v>44408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Roll dates in DATE
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610510AD-BF40-4897-AF40-CEB60CE25377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B284300E-2CB8-4640-B1A1-AC6173D10435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -813,157 +813,187 @@
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50">
+      <c r="B50" s="7">
+        <f>DATE(2019,14,29)</f>
+        <v>43890</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="7">
+        <f>DATE(2020,14,29)</f>
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="7">
+        <f>DATE(2021,14,29)</f>
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="7">
+        <f>DATE(2021,14,-1)</f>
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="7">
+        <f>DATE(2021,-3,-1)</f>
+        <v>44073</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55">
         <f>DATEVALUE("1/15/2021")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56">
         <f>DATEVALUE("2021/01/15")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57">
         <f>DATEVALUE("January 15, 2021")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58">
         <f>DATEVALUE("Jan 2021")</f>
         <v>44197</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59">
         <f>DATEVALUE("1/15")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60">
         <f>DATEVALUE("Jan 15")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61">
         <f>DATEVALUE("JAN-15")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B57">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62">
         <f>DATEVALUE("Jan 2021")</f>
         <v>44197</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B58">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63">
         <f>DATEVALUE("Jan 15, 2021")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B59">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64">
         <f>DATEVALUE("Jan2021")</f>
         <v>44197</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B60">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65">
         <f>DATEVALUE("Jan15")</f>
         <v>44211</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B61">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66">
         <f>DATEVALUE("01 Jan 1985")</f>
         <v>31048</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B62">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67">
         <f>DATEVALUE("01 April 2020")</f>
         <v>43922</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B63" t="e">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="e">
         <f>DATEVALUE("XYZ 20")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B64" s="9">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="9">
         <f>YEARFRAC("2001/01/25","2001/09/27")</f>
         <v>0.67222222222222228</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B65" s="9">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="9">
         <f>YEARFRAC("01/01/2018","12/31/2018")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B66" s="9">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="9">
         <f>YEARFRAC("01/01/2018","07/31/2018")</f>
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B67" s="8">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="8">
         <f>YEARFRAC("1 Jan 20","1 April 2020",0)</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B68" s="9">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="9">
         <f>YEARFRAC("01 Jan 2020","01 April 2020",1)</f>
         <v>0.24863387978142076</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B69" s="9">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="9">
         <f>YEARFRAC("01 Jan 2020","02 Jan 2020",1)</f>
         <v>2.7322404371584699E-3</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B70" s="9">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="9">
         <f>YEARFRAC("01 Jan 1985","02 Jan 1985",1)</f>
         <v>2.7397260273972603E-3</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B71" s="9">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="9">
         <f>YEARFRAC("01 Jan 1985","01 April 2020",1)</f>
         <v>35.247091033538673</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B72" s="9">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="9">
         <f>YEARFRAC("01 Jan 2020","01 April 2020",1)</f>
         <v>0.24863387978142076</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B73" s="9">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="9">
         <f>YEARFRAC("01 Jan 2020","01 April 2020",2)</f>
         <v>0.25277777777777777</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B74" s="9">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="9">
         <f>YEARFRAC("01 Jan 2020","01 April 2020",3)</f>
         <v>0.24931506849315069</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B75" s="9">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="9">
         <f>YEARFRAC("01 Jan 2020","01 April 2020",4)</f>
         <v>0.25</v>
       </c>

</xml_diff>

<commit_message>
Add range metadata. Add initial vlookup
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B284300E-2CB8-4640-B1A1-AC6173D10435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563C108C-9930-48E0-9692-0DCA80F06290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>=1+1</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Tenure (Years)</t>
+  </si>
+  <si>
+    <t>Levy</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
@@ -1006,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525E6BAE-ADD8-5442-95D5-81931F206D16}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1018,7 +1021,7 @@
     <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1027,7 +1030,7 @@
       </c>
       <c r="C1" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1064,8 +1067,11 @@
       <c r="M3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1083,6 +1089,10 @@
       <c r="E4" t="s">
         <v>19</v>
       </c>
+      <c r="F4">
+        <f>VLOOKUP(E4,$L$4:$N$6,2)</f>
+        <v>0.2</v>
+      </c>
       <c r="G4">
         <v>100</v>
       </c>
@@ -1103,8 +1113,11 @@
       <c r="M4" s="6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1122,6 +1135,10 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
+      <c r="F5">
+        <f t="shared" ref="F5" si="0">VLOOKUP(E5,$L$4:$N$6,2)</f>
+        <v>0.1</v>
+      </c>
       <c r="G5">
         <v>200</v>
       </c>
@@ -1133,7 +1150,7 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J6" si="0">SUM(G5:I5)</f>
+        <f t="shared" ref="J5:J6" si="1">SUM(G5:I5)</f>
         <v>229</v>
       </c>
       <c r="L5" t="s">
@@ -1142,8 +1159,11 @@
       <c r="M5" s="6">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1161,6 +1181,10 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
+      <c r="F6">
+        <f>VLOOKUP(E6,$L$4:$N$6,2)</f>
+        <v>0.3</v>
+      </c>
       <c r="G6">
         <v>300</v>
       </c>
@@ -1172,7 +1196,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>340</v>
       </c>
       <c r="L6" t="s">
@@ -1181,18 +1205,21 @@
       <c r="M6" s="6">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G7">
         <f>SUM(G4:G6)</f>
         <v>600</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:I7" si="1">SUM(H4:H6)</f>
+        <f t="shared" ref="H7:I7" si="2">SUM(H4:H6)</f>
         <v>72</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J7">
@@ -1200,13 +1227,13 @@
         <v>687</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H8">
         <f>SUM(G4:G6)-SUM(H4:H6)</f>
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1242,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1223,7 +1250,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1232,7 +1259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
SUMIF WIP - do not merge yet
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563C108C-9930-48E0-9692-0DCA80F06290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7618076-5EF9-4C4A-85C4-1D2BBADF229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>=1+1</t>
   </si>
@@ -79,15 +79,6 @@
     <t>OK?</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -122,6 +113,18 @@
   </si>
   <si>
     <t>Levy</t>
+  </si>
+  <si>
+    <t>Super Tax Amount</t>
+  </si>
+  <si>
+    <t>L's Total</t>
+  </si>
+  <si>
+    <t>L Filter</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -505,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1009,21 +1012,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525E6BAE-ADD8-5442-95D5-81931F206D16}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7">
         <v>44437</v>
@@ -1035,19 +1039,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -1059,16 +1063,16 @@
         <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1087,7 +1091,7 @@
         <v>3.661111111111111</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <f>VLOOKUP(E4,$L$4:$N$6,2)</f>
@@ -1108,7 +1112,7 @@
         <v>118</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M4" s="6">
         <v>0.1</v>
@@ -1133,7 +1137,7 @@
         <v>1.1600547195622435</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5" si="0">VLOOKUP(E5,$L$4:$N$6,2)</f>
@@ -1154,7 +1158,7 @@
         <v>229</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M5" s="6">
         <v>0.2</v>
@@ -1179,7 +1183,7 @@
         <v>0.99178082191780825</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <f>VLOOKUP(E6,$L$4:$N$6,2)</f>
@@ -1200,7 +1204,7 @@
         <v>340</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M6" s="6">
         <v>0.3</v>
@@ -1259,13 +1263,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B14" t="str">
         <f>IF(J7&lt;ALLOWEDTOTAL,"YES","NO")</f>
         <v>YES</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <f>SUMIF(J4:J6,"&gt;200")</f>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <f>SUMIF(J4:J6,"&gt;" &amp; J4)</f>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <f>SUMIF(E4:E6,B12,J4:J6)</f>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f>SUMIF(E4:E6,"L*",J4:J6)</f>
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -1276,156 +1321,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>300</v>
       </c>
       <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <f>SUM(A2:B4)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C6">
-        <f>_xlfn.DAYS(D9,E9)</f>
-        <v>-577</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D9" s="7">
-        <v>43831</v>
-      </c>
-      <c r="E9" s="7">
-        <v>44408</v>
-      </c>
-      <c r="G9">
-        <f>E9-D9</f>
-        <v>577</v>
-      </c>
-      <c r="H9">
-        <f>G9/360</f>
-        <v>1.6027777777777779</v>
-      </c>
-      <c r="J9">
-        <f>570/360</f>
-        <v>1.5833333333333333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G10">
-        <f>DATEDIF(D9,E9,"m")</f>
-        <v>18</v>
-      </c>
-      <c r="H10">
-        <f>G10*30</f>
-        <v>540</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D11">
-        <f>YEARFRAC(D9,E9,0)</f>
-        <v>1.5833333333333333</v>
-      </c>
-      <c r="G11">
-        <f>DATEDIF(D9,E9,"y")</f>
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <f>H10+31</f>
-        <v>571</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G12">
-        <f>DATEDIF(D9,E9,"d")</f>
-        <v>577</v>
-      </c>
-      <c r="H12">
-        <f>H11/360</f>
-        <v>1.586111111111111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G14">
-        <f>DAY(D9)</f>
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <f>DAY(E9)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G15">
-        <f>MONTH(D9)</f>
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <f>MONTH(E9)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G16">
-        <f>YEAR(D9)</f>
-        <v>2020</v>
-      </c>
-      <c r="H16">
-        <f>YEAR(E9)</f>
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="3">
-        <f>D9</f>
-        <v>43831</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G19" s="3">
-        <v>44408</v>
+        <f>SUMIF(A1:A3,"&gt;"&amp;A1)</f>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic SUMIF, refactoring, fixes
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7618076-5EF9-4C4A-85C4-1D2BBADF229A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A3DEDD-A38E-41A0-9B03-4A521722B32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="4284" yWindow="984" windowWidth="15684" windowHeight="11112" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
   <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
@@ -1321,31 +1321,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>300</v>
       </c>
       <c r="B3">
         <f>SUMIF(A1:A3,"&gt;"&amp;A1)</f>
         <v>500</v>
+      </c>
+      <c r="C3">
+        <f>12+12</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamic construction of ranges etc (dates, pmt)
</commit_message>
<xml_diff>
--- a/resources/TEST1.xlsx
+++ b/resources/TEST1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11946AA9-8271-48F9-B023-B42310307A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB391E4-4A43-452A-8E54-953D3BCAA41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="408" windowWidth="15684" windowHeight="11832" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="840" yWindow="168" windowWidth="21756" windowHeight="11832" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +160,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -192,6 +198,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,16 +514,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9E8944-CB9C-0E40-84E2-B10A78E31FE1}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1002,6 +1010,90 @@
       <c r="B80" s="9">
         <f>YEARFRAC("01 Jan 2020","01 April 2020",4)</f>
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="10">
+        <f>DATE(2022,2,1)</f>
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <f>YEAR(DATE(2022,2,1))</f>
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <f>MONTH(DATE(2022,2,1))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <f>DAY(DATE(2022,2,1))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <f>CEILING(-2.5, -1)</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <f>CEILING(2.5, 1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <f>CEILING(-2.5, 1)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="e">
+        <f>CEILING(2.5,-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B89" s="11">
+        <f>CEILING(-2.5, -2)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B90" s="11">
+        <f>CEILING(-2.5, 2)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B91" s="11">
+        <f>CEILING(1.5, 0.1)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B92" s="11">
+        <f>CEILING(0.234, 0.01)</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="7">
+        <f>EOMONTH(DATE(2020,1,15),1)</f>
+        <v>43890</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="7">
+        <f>EDATE(DATE(2020,1,15),1)</f>
+        <v>43876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>